<commit_message>
No more FutureWarnings in performance measures
</commit_message>
<xml_diff>
--- a/Performance Measures.xlsx
+++ b/Performance Measures.xlsx
@@ -573,13 +573,13 @@
         <v>0.0987903671160225</v>
       </c>
       <c r="F5" t="n">
-        <v>0.09950272631738391</v>
+        <v>0.09950272631738398</v>
       </c>
       <c r="G5" t="n">
         <v>0.1060569278364601</v>
       </c>
       <c r="H5" t="n">
-        <v>0.2492855966251572</v>
+        <v>0.2492855966251576</v>
       </c>
     </row>
     <row r="6">
@@ -685,13 +685,13 @@
         <v>0.1717476017549357</v>
       </c>
       <c r="F9" t="n">
-        <v>0.1401294296977708</v>
+        <v>0.1401294296977707</v>
       </c>
       <c r="G9" t="n">
         <v>0.4531597487164368</v>
       </c>
       <c r="H9" t="n">
-        <v>0.001551848031945046</v>
+        <v>0.001551848031945043</v>
       </c>
     </row>
     <row r="10">

</xml_diff>

<commit_message>
Fixed max_drawdown function, syn computing table not working yet
</commit_message>
<xml_diff>
--- a/Performance Measures.xlsx
+++ b/Performance Measures.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Benchmark" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="P1 - Historical" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,7 +441,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>EW - No costs</t>
+          <t>EW</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -451,7 +451,7 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>MVP - No costs</t>
+          <t>MVP</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -461,12 +461,72 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>MSR - No costs</t>
+          <t>MSR</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>MSR - With costs</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Min. risk CVaR</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Min. risk CVaR - With costs</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>Optimal CVaR</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Optimal CVaR - With costs</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Min. risk CDaR</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Min. risk CDaR - With costs</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Optimal CDaR</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Optimal CDaR - With costs</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Min. risk Omega</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Min. risk Omega - With costs</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Optimal Omega</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Optimal Omega - With costs</t>
         </is>
       </c>
     </row>
@@ -477,7 +537,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.04934122451384315</v>
+        <v>0.049341</v>
       </c>
       <c r="C2" t="n">
         <v>0.07511285024057157</v>
@@ -496,6 +556,42 @@
       </c>
       <c r="H2" t="n">
         <v>0.04281234355859342</v>
+      </c>
+      <c r="I2" t="n">
+        <v>0.06695885754874564</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0.06321119010299214</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.07798306381709619</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.03916420041440416</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.06474864412991455</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.06073028485893994</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.07248667530731501</v>
+      </c>
+      <c r="P2" t="n">
+        <v>0.03690580701796131</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>0.06635623267305446</v>
+      </c>
+      <c r="R2" t="n">
+        <v>0.05645993002253635</v>
+      </c>
+      <c r="S2" t="n">
+        <v>0.06846526081957172</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.04784680267269592</v>
       </c>
     </row>
     <row r="3">
@@ -505,7 +601,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.04934122451384315</v>
+        <v>0.049341</v>
       </c>
       <c r="C3" t="n">
         <v>0.07811978622012136</v>
@@ -524,6 +620,42 @@
       </c>
       <c r="H3" t="n">
         <v>0.04289214058796988</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.08275600785723559</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.07616210790152332</v>
+      </c>
+      <c r="K3" t="n">
+        <v>0.08844667140905069</v>
+      </c>
+      <c r="L3" t="n">
+        <v>0.03829555421275314</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0.07652363662261299</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0.07013559032659375</v>
+      </c>
+      <c r="O3" t="n">
+        <v>0.07829719358417983</v>
+      </c>
+      <c r="P3" t="n">
+        <v>0.035955920658406</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>0.08314694127060565</v>
+      </c>
+      <c r="R3" t="n">
+        <v>0.06588454389756243</v>
+      </c>
+      <c r="S3" t="n">
+        <v>0.07346892209824178</v>
+      </c>
+      <c r="T3" t="n">
+        <v>0.04889327672913266</v>
       </c>
     </row>
     <row r="4">
@@ -533,7 +665,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.05639135833150057</v>
+        <v>0.056391</v>
       </c>
       <c r="C4" t="n">
         <v>0.0516408737109758</v>
@@ -552,6 +684,42 @@
       </c>
       <c r="H4" t="n">
         <v>0.04674845873139948</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.03430330156151285</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.03474366819625293</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0.04356993503018398</v>
+      </c>
+      <c r="L4" t="n">
+        <v>0.04453060808782261</v>
+      </c>
+      <c r="M4" t="n">
+        <v>0.03691792969698193</v>
+      </c>
+      <c r="N4" t="n">
+        <v>0.0372511189117369</v>
+      </c>
+      <c r="O4" t="n">
+        <v>0.04725705504243226</v>
+      </c>
+      <c r="P4" t="n">
+        <v>0.04811176851273815</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>0.03313946430072506</v>
+      </c>
+      <c r="R4" t="n">
+        <v>0.03373627663359698</v>
+      </c>
+      <c r="S4" t="n">
+        <v>0.04730205219343551</v>
+      </c>
+      <c r="T4" t="n">
+        <v>0.04726735691315499</v>
       </c>
     </row>
     <row r="5">
@@ -561,7 +729,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.2220354084037478</v>
+        <v>0.222035</v>
       </c>
       <c r="C5" t="n">
         <v>0.152312370186105</v>
@@ -580,6 +748,42 @@
       </c>
       <c r="H5" t="n">
         <v>0.2492855966251576</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.09415936508721523</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.0963954712164433</v>
+      </c>
+      <c r="K5" t="n">
+        <v>0.1049889349555794</v>
+      </c>
+      <c r="L5" t="n">
+        <v>0.2160688388403541</v>
+      </c>
+      <c r="M5" t="n">
+        <v>0.1143676396755364</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.1153442466050348</v>
+      </c>
+      <c r="O5" t="n">
+        <v>0.1239450333778075</v>
+      </c>
+      <c r="P5" t="n">
+        <v>0.2084837940113204</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>0.106304293606713</v>
+      </c>
+      <c r="R5" t="n">
+        <v>0.1082603464732572</v>
+      </c>
+      <c r="S5" t="n">
+        <v>0.1286414685093911</v>
+      </c>
+      <c r="T5" t="n">
+        <v>0.1725324567999956</v>
       </c>
     </row>
     <row r="6">
@@ -589,7 +793,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.07211936324133239</v>
+        <v>0.072119</v>
       </c>
       <c r="C6" t="n">
         <v>0.06358609510140846</v>
@@ -608,6 +812,42 @@
       </c>
       <c r="H6" t="n">
         <v>0.060780642682189</v>
+      </c>
+      <c r="I6" t="n">
+        <v>0.04492404845963597</v>
+      </c>
+      <c r="J6" t="n">
+        <v>0.04614048166376553</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.05663656314976539</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.06076065697738244</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.05368638343389657</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.05433210740825254</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.07748465279634546</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.08146627715198362</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.04875472538176546</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.04971623144676868</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.05940781452605793</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.06109338845926476</v>
       </c>
     </row>
     <row r="7">
@@ -617,7 +857,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.2422591459587894</v>
+        <v>0.242259</v>
       </c>
       <c r="C7" t="n">
         <v>0.1604704890428219</v>
@@ -636,6 +876,42 @@
       </c>
       <c r="H7" t="n">
         <v>0.2739553467247042</v>
+      </c>
+      <c r="I7" t="n">
+        <v>0.08088570093173948</v>
+      </c>
+      <c r="J7" t="n">
+        <v>0.08596300160112007</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.09299025208704255</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.2285944796822431</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.1009561020107799</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.1054672438089822</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.1203048575131326</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.2211003653838322</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.08878711890512607</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.09246353879374736</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.09196459514394932</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.1318487156201701</v>
       </c>
     </row>
     <row r="8">
@@ -645,7 +921,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.1226381935528152</v>
+        <v>0.122638</v>
       </c>
       <c r="C8" t="n">
         <v>0.6329745741220049</v>
@@ -664,6 +940,42 @@
       </c>
       <c r="H8" t="n">
         <v>0.008275211055357412</v>
+      </c>
+      <c r="I8" t="n">
+        <v>0.7151896825054539</v>
+      </c>
+      <c r="J8" t="n">
+        <v>0.5982586464245429</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.8161034345445893</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-0.07323703676451936</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.6046697124422189</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.4913891232699088</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.6361205767952435</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-0.1147262582263156</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.7221221882108834</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.4160044091078337</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.5504998074292227</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.11469463982465</v>
       </c>
     </row>
     <row r="9">
@@ -673,7 +985,7 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.03114698852531302</v>
+        <v>0.031147</v>
       </c>
       <c r="C9" t="n">
         <v>0.2146073887797402</v>
@@ -692,6 +1004,42 @@
       </c>
       <c r="H9" t="n">
         <v>0.001551848031945043</v>
+      </c>
+      <c r="I9" t="n">
+        <v>0.2605515375973824</v>
+      </c>
+      <c r="J9" t="n">
+        <v>0.2156294237126781</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.3386792487804747</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-0.01509375344995455</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.1951876771888221</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.1586970759412157</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.242536423541914</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-0.02647535845312468</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.2251154837217679</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.129636014327044</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.2024212792750599</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.03142198619997644</v>
       </c>
     </row>
     <row r="10">
@@ -721,6 +1069,42 @@
       <c r="H10" t="n">
         <v>0.365271190781277</v>
       </c>
+      <c r="I10" t="n">
+        <v>0.536469699503762</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.5341223780602828</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.4076293411010234</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.4199027069838933</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.519390806571452</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.5184992488839966</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.4995012972617772</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.5028079067912128</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.5535658856193555</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.546271060586925</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.5069561373835163</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.5049264193526888</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
@@ -729,7 +1113,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.6478348465883126</v>
+        <v>0.647835</v>
       </c>
       <c r="C11" t="n">
         <v>0.5554946431602711</v>
@@ -748,6 +1132,42 @@
       </c>
       <c r="H11" t="n">
         <v>0.4217011574688558</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.3774782903158234</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.3774782903158234</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.4020906920724777</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.4020906920724777</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.3805026795179351</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.3805026795179351</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.4039672598077267</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.4039672598077267</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.3927447199451526</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.3927447199451526</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.4297621156472561</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.4297621156472561</v>
       </c>
     </row>
     <row r="12">
@@ -757,7 +1177,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3608590741259927</v>
+        <v>0.360859</v>
       </c>
       <c r="C12" t="n">
         <v>0.2559630748399553</v>
@@ -776,6 +1196,42 @@
       </c>
       <c r="H12" t="n">
         <v>0.2339236433475347</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.2169835055494956</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.2169835055494956</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.2237973887343867</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.2237973887343867</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.2146205699109035</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.2146205699109035</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.2268436095699864</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.2268436095699864</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.2415598577997207</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.2415598577997207</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.2263605968935193</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.2263605968935193</v>
       </c>
     </row>
     <row r="13">
@@ -805,6 +1261,42 @@
       <c r="H13" t="n">
         <v>0.6043766960938161</v>
       </c>
+      <c r="I13" t="n">
+        <v>0.7324409187803218</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.7308367656736235</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.6384585664716415</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.647999002301619</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.7206877316643123</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.7200689195375651</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.706754057124384</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.7090894913839947</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.7440200841505257</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.7391015225169852</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.7120085233924635</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.7105817471288497</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
@@ -832,6 +1324,42 @@
       </c>
       <c r="H14" t="n">
         <v>449.4252735672196</v>
+      </c>
+      <c r="I14" t="n">
+        <v>35.37196486214975</v>
+      </c>
+      <c r="J14" t="n">
+        <v>35.37196486214975</v>
+      </c>
+      <c r="K14" t="n">
+        <v>368.4890547671815</v>
+      </c>
+      <c r="L14" t="n">
+        <v>368.4890547671815</v>
+      </c>
+      <c r="M14" t="n">
+        <v>38.00359170643648</v>
+      </c>
+      <c r="N14" t="n">
+        <v>38.00359170643648</v>
+      </c>
+      <c r="O14" t="n">
+        <v>338.8852096233285</v>
+      </c>
+      <c r="P14" t="n">
+        <v>338.8852096233285</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>93.7022907473345</v>
+      </c>
+      <c r="R14" t="n">
+        <v>93.7022907473345</v>
+      </c>
+      <c r="S14" t="n">
+        <v>195.7782104719494</v>
+      </c>
+      <c r="T14" t="n">
+        <v>195.7782104719494</v>
       </c>
     </row>
   </sheetData>

</xml_diff>